<commit_message>
fix: #abour and .quote
</commit_message>
<xml_diff>
--- a/Lighthouse verdict.xlsx
+++ b/Lighthouse verdict.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sdeor\Projects\OC_Susana\NinaCarducci\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C25D1F42-01E5-43F7-B5F0-F32EBA389AA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC6BC5F7-A2EE-4FD6-8A0F-19B48DFA65DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0A509986-028C-44D6-80D6-665819E5AA6D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{0A509986-028C-44D6-80D6-665819E5AA6D}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,11 +39,111 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+  <si>
+    <t>Performances</t>
+  </si>
+  <si>
+    <t>SEO</t>
+  </si>
+  <si>
+    <t>Le document ne contient pas d'attribut "meta description"</t>
+  </si>
+  <si>
+    <t>Réduisez les ressources JavaScript inutilisées</t>
+  </si>
+  <si>
+    <t>Économies estimées : 526 Kio</t>
+  </si>
+  <si>
+    <t>Réduisez les ressources JavaScript inutilisées et différez le chargement des scripts tant qu'ils ne sont pas requis afin de réduire la quantité d'octets consommés par l'activité réseau.</t>
+  </si>
+  <si>
+    <t>Réduisez les ressources CSS inutilisées</t>
+  </si>
+  <si>
+    <t>Économies estimées : 18 Kio</t>
+  </si>
+  <si>
+    <t>Réduisez les règles inutilisées des feuilles de style et différez les ressources CSS non utilisées pour le contenu au-dessus de la ligne de flottaison afin de réduire la quantité d'octets consommés par l'activité réseau.</t>
+  </si>
+  <si>
+    <t>Réduisez la taille des ressources CSS</t>
+  </si>
+  <si>
+    <t>Économies estimées : 5 Kio</t>
+  </si>
+  <si>
+    <t>La minimisation des fichiers CSS peut réduire la taille des charges utiles de réseau.</t>
+  </si>
+  <si>
+    <t>Réduisez la taille des ressources JavaScript</t>
+  </si>
+  <si>
+    <t>Économies estimées : 15 Kio</t>
+  </si>
+  <si>
+    <t>La minimisation des fichiers JavaScript peut réduire la taille des charges utiles et la durée d'analyse des scripts.</t>
+  </si>
+  <si>
+    <t>Évitez d'utiliser de l'ancien code JavaScript dans les navigateurs récents</t>
+  </si>
+  <si>
+    <t>Économies estimées : 61 Kio</t>
+  </si>
+  <si>
+    <t>Les polyfills et les transformations permettent aux anciens navigateurs d'utiliser les nouvelles fonctionnalités JavaScript. Dans la majorité des cas cependant, ils ne sont pas nécessaires aux navigateurs récents. Envisagez de modifier votre processus de compilation JavaScript pour ne pas transpiler les fonctionnalités Baseline, sauf si vous savez que vous devez prendre en charge les anciens navigateurs.</t>
+  </si>
+  <si>
+    <t>Évitez d'énormes charges utiles de réseau</t>
+  </si>
+  <si>
+    <t>La taille totale était de 30 351 Kio</t>
+  </si>
+  <si>
+    <t>Les charges utiles des grands réseaux coûtent de l'argent réel aux utilisateurs et sont fortement corrélées aux délais de chargement interminables.</t>
+  </si>
+  <si>
+    <t>Le document ne contient pas d'élément &lt;title&gt;</t>
+  </si>
+  <si>
+    <t>Des éléments d'image n'ont pas d'attribut [alt]</t>
+  </si>
+  <si>
+    <t>&lt;meta 
+		name="description" 
+		content="Page de la photographe Nina Carducci. Ses photos, ses tariffs, un formulaire pour la contacter."&gt;</t>
+  </si>
+  <si>
+    <t>&lt;title&gt;Nina Carducci photographie&lt;/title&gt;</t>
+  </si>
+  <si>
+    <t>Toutes les photos ont leur ALT</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
@@ -69,8 +170,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -405,12 +518,160 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED0C0C2B-C6BE-49BC-ACCC-C0B8412AD736}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="A6" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A6" sqref="A1:XFD1048576"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="36.77734375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="36.77734375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="38" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="11.5546875" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+    </row>
+    <row r="2" spans="1:3" ht="55.2" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="69" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="138" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="55.2" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E8E64EC-473B-4611-A99C-C33174B5F3AC}">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="3.77734375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="50.77734375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="3.77734375" style="4"/>
+    <col min="4" max="16384" width="3.77734375" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="3"/>
+    </row>
+    <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="55.2" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="3"/>
+    </row>
+    <row r="6" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="3"/>
+    </row>
+    <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="3"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>